<commit_message>
Third commit - started project within Jupyter Notebook file. Loaded data sources, cleaned datasets, conducted exploratory data analysis, and selected important features
</commit_message>
<xml_diff>
--- a/2020-2021.xlsx
+++ b/2020-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14699\nba-allstar-prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF2E732F-8810-44B7-BAB5-CB41AF05DBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6089EC9F-58BA-4F64-8C5A-4851A6AB4CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{15DF267E-E92A-426B-A747-51B0BC0F951E}"/>
   </bookViews>
@@ -2378,7 +2378,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
@@ -2407,7 +2407,7 @@
     <col min="31" max="31" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="AE16" s="2"/>
     </row>
-    <row r="17" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="AE17" s="2"/>
     </row>
-    <row r="18" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="AE20" s="2"/>
     </row>
-    <row r="21" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="AE23" s="2"/>
     </row>
-    <row r="24" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -4958,7 +4958,7 @@
       </c>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>26</v>
       </c>
@@ -5332,7 +5332,7 @@
       </c>
       <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="AE33" s="2"/>
     </row>
-    <row r="34" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -5613,7 +5613,7 @@
       </c>
       <c r="AE34" s="2"/>
     </row>
-    <row r="35" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>30</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>32</v>
       </c>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="AE37" s="2"/>
     </row>
-    <row r="38" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>34</v>
       </c>
@@ -6084,7 +6084,7 @@
       </c>
       <c r="AE39" s="2"/>
     </row>
-    <row r="40" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>35</v>
       </c>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="AE40" s="2"/>
     </row>
-    <row r="41" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>36</v>
       </c>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="AE41" s="2"/>
     </row>
-    <row r="42" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>37</v>
       </c>
@@ -6363,7 +6363,7 @@
       </c>
       <c r="AE42" s="2"/>
     </row>
-    <row r="43" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>38</v>
       </c>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="AE43" s="2"/>
     </row>
-    <row r="44" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>39</v>
       </c>
@@ -6549,7 +6549,7 @@
       </c>
       <c r="AE44" s="2"/>
     </row>
-    <row r="45" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>40</v>
       </c>
@@ -6642,7 +6642,7 @@
       </c>
       <c r="AE45" s="2"/>
     </row>
-    <row r="46" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>41</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>42</v>
       </c>
@@ -6830,7 +6830,7 @@
       </c>
       <c r="AE47" s="2"/>
     </row>
-    <row r="48" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>42</v>
       </c>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="AE48" s="2"/>
     </row>
-    <row r="49" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>42</v>
       </c>
@@ -7016,7 +7016,7 @@
       </c>
       <c r="AE49" s="2"/>
     </row>
-    <row r="50" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43</v>
       </c>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="AE50" s="2"/>
     </row>
-    <row r="51" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>44</v>
       </c>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="AE51" s="2"/>
     </row>
-    <row r="52" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>44</v>
       </c>
@@ -7295,7 +7295,7 @@
       </c>
       <c r="AE52" s="2"/>
     </row>
-    <row r="53" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>44</v>
       </c>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="AE53" s="2"/>
     </row>
-    <row r="54" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>44</v>
       </c>
@@ -7481,7 +7481,7 @@
       </c>
       <c r="AE54" s="2"/>
     </row>
-    <row r="55" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>45</v>
       </c>
@@ -7574,7 +7574,7 @@
       </c>
       <c r="AE55" s="2"/>
     </row>
-    <row r="56" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>46</v>
       </c>
@@ -7667,7 +7667,7 @@
       </c>
       <c r="AE56" s="2"/>
     </row>
-    <row r="57" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>47</v>
       </c>
@@ -7760,7 +7760,7 @@
       </c>
       <c r="AE57" s="2"/>
     </row>
-    <row r="58" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>48</v>
       </c>
@@ -7853,7 +7853,7 @@
       </c>
       <c r="AE58" s="2"/>
     </row>
-    <row r="59" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>49</v>
       </c>
@@ -7948,7 +7948,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>50</v>
       </c>
@@ -8041,7 +8041,7 @@
       </c>
       <c r="AE60" s="2"/>
     </row>
-    <row r="61" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>51</v>
       </c>
@@ -8134,7 +8134,7 @@
       </c>
       <c r="AE61" s="2"/>
     </row>
-    <row r="62" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>52</v>
       </c>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="AE62" s="2"/>
     </row>
-    <row r="63" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>53</v>
       </c>
@@ -8320,7 +8320,7 @@
       </c>
       <c r="AE63" s="2"/>
     </row>
-    <row r="64" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>54</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>55</v>
       </c>
@@ -8508,7 +8508,7 @@
       </c>
       <c r="AE65" s="2"/>
     </row>
-    <row r="66" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>55</v>
       </c>
@@ -8601,7 +8601,7 @@
       </c>
       <c r="AE66" s="2"/>
     </row>
-    <row r="67" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>55</v>
       </c>
@@ -8694,7 +8694,7 @@
       </c>
       <c r="AE67" s="2"/>
     </row>
-    <row r="68" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>56</v>
       </c>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="AE68" s="2"/>
     </row>
-    <row r="69" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>57</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>58</v>
       </c>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="AE70" s="2"/>
     </row>
-    <row r="71" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>59</v>
       </c>
@@ -9070,7 +9070,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>60</v>
       </c>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="AE72" s="2"/>
     </row>
-    <row r="73" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>61</v>
       </c>
@@ -9256,7 +9256,7 @@
       </c>
       <c r="AE73" s="2"/>
     </row>
-    <row r="74" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>62</v>
       </c>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="AE74" s="2"/>
     </row>
-    <row r="75" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>63</v>
       </c>
@@ -9442,7 +9442,7 @@
       </c>
       <c r="AE75" s="2"/>
     </row>
-    <row r="76" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>64</v>
       </c>
@@ -9535,7 +9535,7 @@
       </c>
       <c r="AE76" s="2"/>
     </row>
-    <row r="77" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>65</v>
       </c>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="AE77" s="2"/>
     </row>
-    <row r="78" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>65</v>
       </c>
@@ -9721,7 +9721,7 @@
       </c>
       <c r="AE78" s="2"/>
     </row>
-    <row r="79" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>65</v>
       </c>
@@ -9814,7 +9814,7 @@
       </c>
       <c r="AE79" s="2"/>
     </row>
-    <row r="80" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>66</v>
       </c>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="AE80" s="2"/>
     </row>
-    <row r="81" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>67</v>
       </c>
@@ -10000,7 +10000,7 @@
       </c>
       <c r="AE81" s="2"/>
     </row>
-    <row r="82" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>68</v>
       </c>
@@ -10095,7 +10095,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>69</v>
       </c>
@@ -10188,7 +10188,7 @@
       </c>
       <c r="AE83" s="2"/>
     </row>
-    <row r="84" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>70</v>
       </c>
@@ -10281,7 +10281,7 @@
       </c>
       <c r="AE84" s="2"/>
     </row>
-    <row r="85" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>71</v>
       </c>
@@ -10374,7 +10374,7 @@
       </c>
       <c r="AE85" s="2"/>
     </row>
-    <row r="86" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>72</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>73</v>
       </c>
@@ -10562,7 +10562,7 @@
       </c>
       <c r="AE87" s="2"/>
     </row>
-    <row r="88" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>74</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>75</v>
       </c>
@@ -10750,7 +10750,7 @@
       </c>
       <c r="AE89" s="2"/>
     </row>
-    <row r="90" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>76</v>
       </c>
@@ -10843,7 +10843,7 @@
       </c>
       <c r="AE90" s="2"/>
     </row>
-    <row r="91" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>77</v>
       </c>
@@ -10936,7 +10936,7 @@
       </c>
       <c r="AE91" s="2"/>
     </row>
-    <row r="92" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>78</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>79</v>
       </c>
@@ -11124,7 +11124,7 @@
       </c>
       <c r="AE93" s="2"/>
     </row>
-    <row r="94" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>80</v>
       </c>
@@ -11217,7 +11217,7 @@
       </c>
       <c r="AE94" s="2"/>
     </row>
-    <row r="95" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>81</v>
       </c>
@@ -11310,7 +11310,7 @@
       </c>
       <c r="AE95" s="2"/>
     </row>
-    <row r="96" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>82</v>
       </c>
@@ -11403,7 +11403,7 @@
       </c>
       <c r="AE96" s="2"/>
     </row>
-    <row r="97" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>83</v>
       </c>
@@ -11496,7 +11496,7 @@
       </c>
       <c r="AE97" s="2"/>
     </row>
-    <row r="98" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>84</v>
       </c>
@@ -11589,7 +11589,7 @@
       </c>
       <c r="AE98" s="2"/>
     </row>
-    <row r="99" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>85</v>
       </c>
@@ -11682,7 +11682,7 @@
       </c>
       <c r="AE99" s="2"/>
     </row>
-    <row r="100" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>85</v>
       </c>
@@ -11775,7 +11775,7 @@
       </c>
       <c r="AE100" s="2"/>
     </row>
-    <row r="101" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>85</v>
       </c>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="AE101" s="2"/>
     </row>
-    <row r="102" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>86</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>87</v>
       </c>
@@ -12054,7 +12054,7 @@
       </c>
       <c r="AE103" s="2"/>
     </row>
-    <row r="104" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>88</v>
       </c>
@@ -12147,7 +12147,7 @@
       </c>
       <c r="AE104" s="2"/>
     </row>
-    <row r="105" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>89</v>
       </c>
@@ -12240,7 +12240,7 @@
       </c>
       <c r="AE105" s="2"/>
     </row>
-    <row r="106" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>90</v>
       </c>
@@ -12333,7 +12333,7 @@
       </c>
       <c r="AE106" s="2"/>
     </row>
-    <row r="107" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>90</v>
       </c>
@@ -12426,7 +12426,7 @@
       </c>
       <c r="AE107" s="2"/>
     </row>
-    <row r="108" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>90</v>
       </c>
@@ -12517,7 +12517,7 @@
       </c>
       <c r="AE108" s="2"/>
     </row>
-    <row r="109" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>91</v>
       </c>
@@ -12610,7 +12610,7 @@
       </c>
       <c r="AE109" s="2"/>
     </row>
-    <row r="110" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>92</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>92</v>
       </c>
@@ -12798,7 +12798,7 @@
       </c>
       <c r="AE111" s="2"/>
     </row>
-    <row r="112" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>92</v>
       </c>
@@ -12891,7 +12891,7 @@
       </c>
       <c r="AE112" s="2"/>
     </row>
-    <row r="113" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>93</v>
       </c>
@@ -12984,7 +12984,7 @@
       </c>
       <c r="AE113" s="2"/>
     </row>
-    <row r="114" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>94</v>
       </c>
@@ -13077,7 +13077,7 @@
       </c>
       <c r="AE114" s="2"/>
     </row>
-    <row r="115" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>95</v>
       </c>
@@ -13170,7 +13170,7 @@
       </c>
       <c r="AE115" s="2"/>
     </row>
-    <row r="116" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>96</v>
       </c>
@@ -13263,7 +13263,7 @@
       </c>
       <c r="AE116" s="2"/>
     </row>
-    <row r="117" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>97</v>
       </c>
@@ -13356,7 +13356,7 @@
       </c>
       <c r="AE117" s="2"/>
     </row>
-    <row r="118" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>98</v>
       </c>
@@ -13451,7 +13451,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>99</v>
       </c>
@@ -13546,7 +13546,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="120" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>100</v>
       </c>
@@ -13639,7 +13639,7 @@
       </c>
       <c r="AE120" s="2"/>
     </row>
-    <row r="121" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>101</v>
       </c>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="AE121" s="2"/>
     </row>
-    <row r="122" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>102</v>
       </c>
@@ -13825,7 +13825,7 @@
       </c>
       <c r="AE122" s="2"/>
     </row>
-    <row r="123" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>103</v>
       </c>
@@ -13918,7 +13918,7 @@
       </c>
       <c r="AE123" s="2"/>
     </row>
-    <row r="124" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>104</v>
       </c>
@@ -14011,7 +14011,7 @@
       </c>
       <c r="AE124" s="2"/>
     </row>
-    <row r="125" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>105</v>
       </c>
@@ -14104,7 +14104,7 @@
       </c>
       <c r="AE125" s="2"/>
     </row>
-    <row r="126" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>106</v>
       </c>
@@ -14197,7 +14197,7 @@
       </c>
       <c r="AE126" s="2"/>
     </row>
-    <row r="127" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>107</v>
       </c>
@@ -14292,7 +14292,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>108</v>
       </c>
@@ -14385,7 +14385,7 @@
       </c>
       <c r="AE128" s="2"/>
     </row>
-    <row r="129" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>109</v>
       </c>
@@ -14478,7 +14478,7 @@
       </c>
       <c r="AE129" s="2"/>
     </row>
-    <row r="130" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>110</v>
       </c>
@@ -14571,7 +14571,7 @@
       </c>
       <c r="AE130" s="2"/>
     </row>
-    <row r="131" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>110</v>
       </c>
@@ -14664,7 +14664,7 @@
       </c>
       <c r="AE131" s="2"/>
     </row>
-    <row r="132" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>110</v>
       </c>
@@ -14757,7 +14757,7 @@
       </c>
       <c r="AE132" s="2"/>
     </row>
-    <row r="133" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>111</v>
       </c>
@@ -14850,7 +14850,7 @@
       </c>
       <c r="AE133" s="2"/>
     </row>
-    <row r="134" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>111</v>
       </c>
@@ -14943,7 +14943,7 @@
       </c>
       <c r="AE134" s="2"/>
     </row>
-    <row r="135" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>111</v>
       </c>
@@ -15036,7 +15036,7 @@
       </c>
       <c r="AE135" s="2"/>
     </row>
-    <row r="136" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>112</v>
       </c>
@@ -15129,7 +15129,7 @@
       </c>
       <c r="AE136" s="2"/>
     </row>
-    <row r="137" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>113</v>
       </c>
@@ -15224,7 +15224,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="138" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>114</v>
       </c>
@@ -15319,7 +15319,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="139" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>115</v>
       </c>
@@ -15412,7 +15412,7 @@
       </c>
       <c r="AE139" s="2"/>
     </row>
-    <row r="140" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>116</v>
       </c>
@@ -15505,7 +15505,7 @@
       </c>
       <c r="AE140" s="2"/>
     </row>
-    <row r="141" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>117</v>
       </c>
@@ -15598,7 +15598,7 @@
       </c>
       <c r="AE141" s="2"/>
     </row>
-    <row r="142" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>118</v>
       </c>
@@ -15691,7 +15691,7 @@
       </c>
       <c r="AE142" s="2"/>
     </row>
-    <row r="143" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>119</v>
       </c>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="AE143" s="2"/>
     </row>
-    <row r="144" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>120</v>
       </c>
@@ -15877,7 +15877,7 @@
       </c>
       <c r="AE144" s="2"/>
     </row>
-    <row r="145" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>121</v>
       </c>
@@ -15972,7 +15972,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="146" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>122</v>
       </c>
@@ -16067,7 +16067,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="147" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>123</v>
       </c>
@@ -16160,7 +16160,7 @@
       </c>
       <c r="AE147" s="2"/>
     </row>
-    <row r="148" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>124</v>
       </c>
@@ -16253,7 +16253,7 @@
       </c>
       <c r="AE148" s="2"/>
     </row>
-    <row r="149" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>125</v>
       </c>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="AE149" s="2"/>
     </row>
-    <row r="150" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>126</v>
       </c>
@@ -16439,7 +16439,7 @@
       </c>
       <c r="AE150" s="2"/>
     </row>
-    <row r="151" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>127</v>
       </c>
@@ -16532,7 +16532,7 @@
       </c>
       <c r="AE151" s="2"/>
     </row>
-    <row r="152" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>127</v>
       </c>
@@ -16623,7 +16623,7 @@
       </c>
       <c r="AE152" s="2"/>
     </row>
-    <row r="153" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>127</v>
       </c>
@@ -16716,7 +16716,7 @@
       </c>
       <c r="AE153" s="2"/>
     </row>
-    <row r="154" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>128</v>
       </c>
@@ -16809,7 +16809,7 @@
       </c>
       <c r="AE154" s="2"/>
     </row>
-    <row r="155" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>129</v>
       </c>
@@ -16902,7 +16902,7 @@
       </c>
       <c r="AE155" s="2"/>
     </row>
-    <row r="156" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>130</v>
       </c>
@@ -16997,7 +16997,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="157" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>131</v>
       </c>
@@ -17090,7 +17090,7 @@
       </c>
       <c r="AE157" s="2"/>
     </row>
-    <row r="158" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>132</v>
       </c>
@@ -17185,7 +17185,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="159" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>133</v>
       </c>
@@ -17280,7 +17280,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="160" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>134</v>
       </c>
@@ -17373,7 +17373,7 @@
       </c>
       <c r="AE160" s="2"/>
     </row>
-    <row r="161" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>135</v>
       </c>
@@ -17466,7 +17466,7 @@
       </c>
       <c r="AE161" s="2"/>
     </row>
-    <row r="162" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>135</v>
       </c>
@@ -17559,7 +17559,7 @@
       </c>
       <c r="AE162" s="2"/>
     </row>
-    <row r="163" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>135</v>
       </c>
@@ -17652,7 +17652,7 @@
       </c>
       <c r="AE163" s="2"/>
     </row>
-    <row r="164" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>136</v>
       </c>
@@ -17745,7 +17745,7 @@
       </c>
       <c r="AE164" s="2"/>
     </row>
-    <row r="165" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>137</v>
       </c>
@@ -17838,7 +17838,7 @@
       </c>
       <c r="AE165" s="2"/>
     </row>
-    <row r="166" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>138</v>
       </c>
@@ -17933,7 +17933,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="167" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>139</v>
       </c>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="AE167" s="2"/>
     </row>
-    <row r="168" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>140</v>
       </c>
@@ -18119,7 +18119,7 @@
       </c>
       <c r="AE168" s="2"/>
     </row>
-    <row r="169" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>141</v>
       </c>
@@ -18214,7 +18214,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="170" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>142</v>
       </c>
@@ -18307,7 +18307,7 @@
       </c>
       <c r="AE170" s="2"/>
     </row>
-    <row r="171" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>143</v>
       </c>
@@ -18402,7 +18402,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="172" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>144</v>
       </c>
@@ -18495,7 +18495,7 @@
       </c>
       <c r="AE172" s="2"/>
     </row>
-    <row r="173" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>145</v>
       </c>
@@ -18588,7 +18588,7 @@
       </c>
       <c r="AE173" s="2"/>
     </row>
-    <row r="174" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>146</v>
       </c>
@@ -18681,7 +18681,7 @@
       </c>
       <c r="AE174" s="2"/>
     </row>
-    <row r="175" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>147</v>
       </c>
@@ -18774,7 +18774,7 @@
       </c>
       <c r="AE175" s="2"/>
     </row>
-    <row r="176" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>147</v>
       </c>
@@ -18867,7 +18867,7 @@
       </c>
       <c r="AE176" s="2"/>
     </row>
-    <row r="177" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>147</v>
       </c>
@@ -18960,7 +18960,7 @@
       </c>
       <c r="AE177" s="2"/>
     </row>
-    <row r="178" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>148</v>
       </c>
@@ -19053,7 +19053,7 @@
       </c>
       <c r="AE178" s="2"/>
     </row>
-    <row r="179" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>149</v>
       </c>
@@ -19146,7 +19146,7 @@
       </c>
       <c r="AE179" s="2"/>
     </row>
-    <row r="180" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>150</v>
       </c>
@@ -19239,7 +19239,7 @@
       </c>
       <c r="AE180" s="2"/>
     </row>
-    <row r="181" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>151</v>
       </c>
@@ -19332,7 +19332,7 @@
       </c>
       <c r="AE181" s="2"/>
     </row>
-    <row r="182" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>152</v>
       </c>
@@ -19427,7 +19427,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="183" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>153</v>
       </c>
@@ -19520,7 +19520,7 @@
       </c>
       <c r="AE183" s="2"/>
     </row>
-    <row r="184" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>154</v>
       </c>
@@ -19613,7 +19613,7 @@
       </c>
       <c r="AE184" s="2"/>
     </row>
-    <row r="185" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>154</v>
       </c>
@@ -19706,7 +19706,7 @@
       </c>
       <c r="AE185" s="2"/>
     </row>
-    <row r="186" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>154</v>
       </c>
@@ -19799,7 +19799,7 @@
       </c>
       <c r="AE186" s="2"/>
     </row>
-    <row r="187" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>155</v>
       </c>
@@ -19892,7 +19892,7 @@
       </c>
       <c r="AE187" s="2"/>
     </row>
-    <row r="188" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>156</v>
       </c>
@@ -19985,7 +19985,7 @@
       </c>
       <c r="AE188" s="2"/>
     </row>
-    <row r="189" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>156</v>
       </c>
@@ -20078,7 +20078,7 @@
       </c>
       <c r="AE189" s="2"/>
     </row>
-    <row r="190" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>156</v>
       </c>
@@ -20171,7 +20171,7 @@
       </c>
       <c r="AE190" s="2"/>
     </row>
-    <row r="191" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>157</v>
       </c>
@@ -20264,7 +20264,7 @@
       </c>
       <c r="AE191" s="2"/>
     </row>
-    <row r="192" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>158</v>
       </c>
@@ -20359,7 +20359,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="193" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>159</v>
       </c>
@@ -20452,7 +20452,7 @@
       </c>
       <c r="AE193" s="2"/>
     </row>
-    <row r="194" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>160</v>
       </c>
@@ -20545,7 +20545,7 @@
       </c>
       <c r="AE194" s="2"/>
     </row>
-    <row r="195" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>161</v>
       </c>
@@ -20638,7 +20638,7 @@
       </c>
       <c r="AE195" s="2"/>
     </row>
-    <row r="196" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>162</v>
       </c>
@@ -20731,7 +20731,7 @@
       </c>
       <c r="AE196" s="2"/>
     </row>
-    <row r="197" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>163</v>
       </c>
@@ -20824,7 +20824,7 @@
       </c>
       <c r="AE197" s="2"/>
     </row>
-    <row r="198" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>163</v>
       </c>
@@ -20917,7 +20917,7 @@
       </c>
       <c r="AE198" s="2"/>
     </row>
-    <row r="199" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>163</v>
       </c>
@@ -21010,7 +21010,7 @@
       </c>
       <c r="AE199" s="2"/>
     </row>
-    <row r="200" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>164</v>
       </c>
@@ -21103,7 +21103,7 @@
       </c>
       <c r="AE200" s="2"/>
     </row>
-    <row r="201" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>165</v>
       </c>
@@ -21196,7 +21196,7 @@
       </c>
       <c r="AE201" s="2"/>
     </row>
-    <row r="202" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>166</v>
       </c>
@@ -21289,7 +21289,7 @@
       </c>
       <c r="AE202" s="2"/>
     </row>
-    <row r="203" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>167</v>
       </c>
@@ -21382,7 +21382,7 @@
       </c>
       <c r="AE203" s="2"/>
     </row>
-    <row r="204" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>168</v>
       </c>
@@ -21475,7 +21475,7 @@
       </c>
       <c r="AE204" s="2"/>
     </row>
-    <row r="205" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>169</v>
       </c>
@@ -21568,7 +21568,7 @@
       </c>
       <c r="AE205" s="2"/>
     </row>
-    <row r="206" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>170</v>
       </c>
@@ -21661,7 +21661,7 @@
       </c>
       <c r="AE206" s="2"/>
     </row>
-    <row r="207" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>171</v>
       </c>
@@ -21754,7 +21754,7 @@
       </c>
       <c r="AE207" s="2"/>
     </row>
-    <row r="208" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>172</v>
       </c>
@@ -21847,7 +21847,7 @@
       </c>
       <c r="AE208" s="2"/>
     </row>
-    <row r="209" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>173</v>
       </c>
@@ -21940,7 +21940,7 @@
       </c>
       <c r="AE209" s="2"/>
     </row>
-    <row r="210" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>174</v>
       </c>
@@ -22033,7 +22033,7 @@
       </c>
       <c r="AE210" s="2"/>
     </row>
-    <row r="211" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>175</v>
       </c>
@@ -22126,7 +22126,7 @@
       </c>
       <c r="AE211" s="2"/>
     </row>
-    <row r="212" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>176</v>
       </c>
@@ -22219,7 +22219,7 @@
       </c>
       <c r="AE212" s="2"/>
     </row>
-    <row r="213" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>177</v>
       </c>
@@ -22312,7 +22312,7 @@
       </c>
       <c r="AE213" s="2"/>
     </row>
-    <row r="214" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
         <v>178</v>
       </c>
@@ -22405,7 +22405,7 @@
       </c>
       <c r="AE214" s="2"/>
     </row>
-    <row r="215" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
         <v>179</v>
       </c>
@@ -22498,7 +22498,7 @@
       </c>
       <c r="AE215" s="2"/>
     </row>
-    <row r="216" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A216" s="1">
         <v>179</v>
       </c>
@@ -22591,7 +22591,7 @@
       </c>
       <c r="AE216" s="2"/>
     </row>
-    <row r="217" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A217" s="1">
         <v>179</v>
       </c>
@@ -22684,7 +22684,7 @@
       </c>
       <c r="AE217" s="2"/>
     </row>
-    <row r="218" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A218" s="1">
         <v>180</v>
       </c>
@@ -22777,7 +22777,7 @@
       </c>
       <c r="AE218" s="2"/>
     </row>
-    <row r="219" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A219" s="1">
         <v>181</v>
       </c>
@@ -22870,7 +22870,7 @@
       </c>
       <c r="AE219" s="2"/>
     </row>
-    <row r="220" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A220" s="1">
         <v>182</v>
       </c>
@@ -22963,7 +22963,7 @@
       </c>
       <c r="AE220" s="2"/>
     </row>
-    <row r="221" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A221" s="1">
         <v>183</v>
       </c>
@@ -23056,7 +23056,7 @@
       </c>
       <c r="AE221" s="2"/>
     </row>
-    <row r="222" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A222" s="1">
         <v>184</v>
       </c>
@@ -23149,7 +23149,7 @@
       </c>
       <c r="AE222" s="2"/>
     </row>
-    <row r="223" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A223" s="1">
         <v>185</v>
       </c>
@@ -23242,7 +23242,7 @@
       </c>
       <c r="AE223" s="2"/>
     </row>
-    <row r="224" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A224" s="1">
         <v>186</v>
       </c>
@@ -23335,7 +23335,7 @@
       </c>
       <c r="AE224" s="2"/>
     </row>
-    <row r="225" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A225" s="1">
         <v>186</v>
       </c>
@@ -23428,7 +23428,7 @@
       </c>
       <c r="AE225" s="2"/>
     </row>
-    <row r="226" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>186</v>
       </c>
@@ -23521,7 +23521,7 @@
       </c>
       <c r="AE226" s="2"/>
     </row>
-    <row r="227" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A227" s="1">
         <v>187</v>
       </c>
@@ -23614,7 +23614,7 @@
       </c>
       <c r="AE227" s="2"/>
     </row>
-    <row r="228" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A228" s="1">
         <v>188</v>
       </c>
@@ -23707,7 +23707,7 @@
       </c>
       <c r="AE228" s="2"/>
     </row>
-    <row r="229" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A229" s="1">
         <v>189</v>
       </c>
@@ -23800,7 +23800,7 @@
       </c>
       <c r="AE229" s="2"/>
     </row>
-    <row r="230" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A230" s="1">
         <v>189</v>
       </c>
@@ -23893,7 +23893,7 @@
       </c>
       <c r="AE230" s="2"/>
     </row>
-    <row r="231" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A231" s="1">
         <v>189</v>
       </c>
@@ -23986,7 +23986,7 @@
       </c>
       <c r="AE231" s="2"/>
     </row>
-    <row r="232" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A232" s="1">
         <v>190</v>
       </c>
@@ -24081,7 +24081,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="233" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A233" s="1">
         <v>191</v>
       </c>
@@ -24174,7 +24174,7 @@
       </c>
       <c r="AE233" s="2"/>
     </row>
-    <row r="234" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A234" s="1">
         <v>192</v>
       </c>
@@ -24267,7 +24267,7 @@
       </c>
       <c r="AE234" s="2"/>
     </row>
-    <row r="235" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A235" s="1">
         <v>192</v>
       </c>
@@ -24360,7 +24360,7 @@
       </c>
       <c r="AE235" s="2"/>
     </row>
-    <row r="236" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A236" s="1">
         <v>192</v>
       </c>
@@ -24453,7 +24453,7 @@
       </c>
       <c r="AE236" s="2"/>
     </row>
-    <row r="237" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A237" s="1">
         <v>193</v>
       </c>
@@ -24546,7 +24546,7 @@
       </c>
       <c r="AE237" s="2"/>
     </row>
-    <row r="238" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A238" s="1">
         <v>194</v>
       </c>
@@ -24639,7 +24639,7 @@
       </c>
       <c r="AE238" s="2"/>
     </row>
-    <row r="239" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A239" s="1">
         <v>195</v>
       </c>
@@ -24732,7 +24732,7 @@
       </c>
       <c r="AE239" s="2"/>
     </row>
-    <row r="240" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A240" s="1">
         <v>196</v>
       </c>
@@ -24825,7 +24825,7 @@
       </c>
       <c r="AE240" s="2"/>
     </row>
-    <row r="241" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A241" s="1">
         <v>196</v>
       </c>
@@ -24918,7 +24918,7 @@
       </c>
       <c r="AE241" s="2"/>
     </row>
-    <row r="242" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>196</v>
       </c>
@@ -25011,7 +25011,7 @@
       </c>
       <c r="AE242" s="2"/>
     </row>
-    <row r="243" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A243" s="1">
         <v>197</v>
       </c>
@@ -25104,7 +25104,7 @@
       </c>
       <c r="AE243" s="2"/>
     </row>
-    <row r="244" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A244" s="1">
         <v>198</v>
       </c>
@@ -25197,7 +25197,7 @@
       </c>
       <c r="AE244" s="2"/>
     </row>
-    <row r="245" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A245" s="1">
         <v>199</v>
       </c>
@@ -25290,7 +25290,7 @@
       </c>
       <c r="AE245" s="2"/>
     </row>
-    <row r="246" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A246" s="1">
         <v>200</v>
       </c>
@@ -25383,7 +25383,7 @@
       </c>
       <c r="AE246" s="2"/>
     </row>
-    <row r="247" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A247" s="1">
         <v>201</v>
       </c>
@@ -25476,7 +25476,7 @@
       </c>
       <c r="AE247" s="2"/>
     </row>
-    <row r="248" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A248" s="1">
         <v>202</v>
       </c>
@@ -25569,7 +25569,7 @@
       </c>
       <c r="AE248" s="2"/>
     </row>
-    <row r="249" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A249" s="1">
         <v>203</v>
       </c>
@@ -25662,7 +25662,7 @@
       </c>
       <c r="AE249" s="2"/>
     </row>
-    <row r="250" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A250" s="1">
         <v>204</v>
       </c>
@@ -25755,7 +25755,7 @@
       </c>
       <c r="AE250" s="2"/>
     </row>
-    <row r="251" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A251" s="1">
         <v>205</v>
       </c>
@@ -25848,7 +25848,7 @@
       </c>
       <c r="AE251" s="2"/>
     </row>
-    <row r="252" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A252" s="1">
         <v>206</v>
       </c>
@@ -25941,7 +25941,7 @@
       </c>
       <c r="AE252" s="2"/>
     </row>
-    <row r="253" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A253" s="1">
         <v>207</v>
       </c>
@@ -26034,7 +26034,7 @@
       </c>
       <c r="AE253" s="2"/>
     </row>
-    <row r="254" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A254" s="1">
         <v>208</v>
       </c>
@@ -26127,7 +26127,7 @@
       </c>
       <c r="AE254" s="2"/>
     </row>
-    <row r="255" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A255" s="1">
         <v>209</v>
       </c>
@@ -26220,7 +26220,7 @@
       </c>
       <c r="AE255" s="2"/>
     </row>
-    <row r="256" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A256" s="1">
         <v>210</v>
       </c>
@@ -26313,7 +26313,7 @@
       </c>
       <c r="AE256" s="2"/>
     </row>
-    <row r="257" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A257" s="1">
         <v>211</v>
       </c>
@@ -26406,7 +26406,7 @@
       </c>
       <c r="AE257" s="2"/>
     </row>
-    <row r="258" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A258" s="1">
         <v>212</v>
       </c>
@@ -26499,7 +26499,7 @@
       </c>
       <c r="AE258" s="2"/>
     </row>
-    <row r="259" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A259" s="1">
         <v>213</v>
       </c>
@@ -26592,7 +26592,7 @@
       </c>
       <c r="AE259" s="2"/>
     </row>
-    <row r="260" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A260" s="1">
         <v>214</v>
       </c>
@@ -26685,7 +26685,7 @@
       </c>
       <c r="AE260" s="2"/>
     </row>
-    <row r="261" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A261" s="1">
         <v>215</v>
       </c>
@@ -26778,7 +26778,7 @@
       </c>
       <c r="AE261" s="2"/>
     </row>
-    <row r="262" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A262" s="1">
         <v>215</v>
       </c>
@@ -26871,7 +26871,7 @@
       </c>
       <c r="AE262" s="2"/>
     </row>
-    <row r="263" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A263" s="1">
         <v>215</v>
       </c>
@@ -26964,7 +26964,7 @@
       </c>
       <c r="AE263" s="2"/>
     </row>
-    <row r="264" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A264" s="1">
         <v>216</v>
       </c>
@@ -27057,7 +27057,7 @@
       </c>
       <c r="AE264" s="2"/>
     </row>
-    <row r="265" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A265" s="1">
         <v>217</v>
       </c>
@@ -27150,7 +27150,7 @@
       </c>
       <c r="AE265" s="2"/>
     </row>
-    <row r="266" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A266" s="1">
         <v>218</v>
       </c>
@@ -27243,7 +27243,7 @@
       </c>
       <c r="AE266" s="2"/>
     </row>
-    <row r="267" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A267" s="1">
         <v>219</v>
       </c>
@@ -27336,7 +27336,7 @@
       </c>
       <c r="AE267" s="2"/>
     </row>
-    <row r="268" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A268" s="1">
         <v>220</v>
       </c>
@@ -27429,7 +27429,7 @@
       </c>
       <c r="AE268" s="2"/>
     </row>
-    <row r="269" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A269" s="1">
         <v>220</v>
       </c>
@@ -27522,7 +27522,7 @@
       </c>
       <c r="AE269" s="2"/>
     </row>
-    <row r="270" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A270" s="1">
         <v>220</v>
       </c>
@@ -27615,7 +27615,7 @@
       </c>
       <c r="AE270" s="2"/>
     </row>
-    <row r="271" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A271" s="1">
         <v>221</v>
       </c>
@@ -27708,7 +27708,7 @@
       </c>
       <c r="AE271" s="2"/>
     </row>
-    <row r="272" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A272" s="1">
         <v>221</v>
       </c>
@@ -27801,7 +27801,7 @@
       </c>
       <c r="AE272" s="2"/>
     </row>
-    <row r="273" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A273" s="1">
         <v>221</v>
       </c>
@@ -27894,7 +27894,7 @@
       </c>
       <c r="AE273" s="2"/>
     </row>
-    <row r="274" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A274" s="1">
         <v>222</v>
       </c>
@@ -27987,7 +27987,7 @@
       </c>
       <c r="AE274" s="2"/>
     </row>
-    <row r="275" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A275" s="1">
         <v>223</v>
       </c>
@@ -28080,7 +28080,7 @@
       </c>
       <c r="AE275" s="2"/>
     </row>
-    <row r="276" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A276" s="1">
         <v>224</v>
       </c>
@@ -28173,7 +28173,7 @@
       </c>
       <c r="AE276" s="2"/>
     </row>
-    <row r="277" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A277" s="1">
         <v>225</v>
       </c>
@@ -28264,7 +28264,7 @@
       </c>
       <c r="AE277" s="2"/>
     </row>
-    <row r="278" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A278" s="1">
         <v>226</v>
       </c>
@@ -28359,7 +28359,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="279" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A279" s="1">
         <v>227</v>
       </c>
@@ -28450,7 +28450,7 @@
       </c>
       <c r="AE279" s="2"/>
     </row>
-    <row r="280" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A280" s="1">
         <v>228</v>
       </c>
@@ -28543,7 +28543,7 @@
       </c>
       <c r="AE280" s="2"/>
     </row>
-    <row r="281" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A281" s="1">
         <v>229</v>
       </c>
@@ -28636,7 +28636,7 @@
       </c>
       <c r="AE281" s="2"/>
     </row>
-    <row r="282" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A282" s="1">
         <v>229</v>
       </c>
@@ -28729,7 +28729,7 @@
       </c>
       <c r="AE282" s="2"/>
     </row>
-    <row r="283" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A283" s="1">
         <v>229</v>
       </c>
@@ -28822,7 +28822,7 @@
       </c>
       <c r="AE283" s="2"/>
     </row>
-    <row r="284" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A284" s="1">
         <v>230</v>
       </c>
@@ -28915,7 +28915,7 @@
       </c>
       <c r="AE284" s="2"/>
     </row>
-    <row r="285" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A285" s="1">
         <v>231</v>
       </c>
@@ -29008,7 +29008,7 @@
       </c>
       <c r="AE285" s="2"/>
     </row>
-    <row r="286" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A286" s="1">
         <v>232</v>
       </c>
@@ -29101,7 +29101,7 @@
       </c>
       <c r="AE286" s="2"/>
     </row>
-    <row r="287" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A287" s="1">
         <v>233</v>
       </c>
@@ -29194,7 +29194,7 @@
       </c>
       <c r="AE287" s="2"/>
     </row>
-    <row r="288" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A288" s="1">
         <v>234</v>
       </c>
@@ -29287,7 +29287,7 @@
       </c>
       <c r="AE288" s="2"/>
     </row>
-    <row r="289" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A289" s="1">
         <v>235</v>
       </c>
@@ -29378,7 +29378,7 @@
       </c>
       <c r="AE289" s="2"/>
     </row>
-    <row r="290" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A290" s="1">
         <v>236</v>
       </c>
@@ -29471,7 +29471,7 @@
       </c>
       <c r="AE290" s="2"/>
     </row>
-    <row r="291" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A291" s="1">
         <v>236</v>
       </c>
@@ -29564,7 +29564,7 @@
       </c>
       <c r="AE291" s="2"/>
     </row>
-    <row r="292" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A292" s="1">
         <v>236</v>
       </c>
@@ -29657,7 +29657,7 @@
       </c>
       <c r="AE292" s="2"/>
     </row>
-    <row r="293" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A293" s="1">
         <v>237</v>
       </c>
@@ -29750,7 +29750,7 @@
       </c>
       <c r="AE293" s="2"/>
     </row>
-    <row r="294" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A294" s="1">
         <v>238</v>
       </c>
@@ -29843,7 +29843,7 @@
       </c>
       <c r="AE294" s="2"/>
     </row>
-    <row r="295" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A295" s="1">
         <v>239</v>
       </c>
@@ -29936,7 +29936,7 @@
       </c>
       <c r="AE295" s="2"/>
     </row>
-    <row r="296" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A296" s="1">
         <v>240</v>
       </c>
@@ -30029,7 +30029,7 @@
       </c>
       <c r="AE296" s="2"/>
     </row>
-    <row r="297" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A297" s="1">
         <v>241</v>
       </c>
@@ -30122,7 +30122,7 @@
       </c>
       <c r="AE297" s="2"/>
     </row>
-    <row r="298" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A298" s="1">
         <v>242</v>
       </c>
@@ -30215,7 +30215,7 @@
       </c>
       <c r="AE298" s="2"/>
     </row>
-    <row r="299" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A299" s="1">
         <v>243</v>
       </c>
@@ -30308,7 +30308,7 @@
       </c>
       <c r="AE299" s="2"/>
     </row>
-    <row r="300" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A300" s="1">
         <v>244</v>
       </c>
@@ -30401,7 +30401,7 @@
       </c>
       <c r="AE300" s="2"/>
     </row>
-    <row r="301" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A301" s="1">
         <v>245</v>
       </c>
@@ -30494,7 +30494,7 @@
       </c>
       <c r="AE301" s="2"/>
     </row>
-    <row r="302" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A302" s="1">
         <v>246</v>
       </c>
@@ -30587,7 +30587,7 @@
       </c>
       <c r="AE302" s="2"/>
     </row>
-    <row r="303" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A303" s="1">
         <v>246</v>
       </c>
@@ -30680,7 +30680,7 @@
       </c>
       <c r="AE303" s="2"/>
     </row>
-    <row r="304" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A304" s="1">
         <v>246</v>
       </c>
@@ -30773,7 +30773,7 @@
       </c>
       <c r="AE304" s="2"/>
     </row>
-    <row r="305" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A305" s="1">
         <v>247</v>
       </c>
@@ -30866,7 +30866,7 @@
       </c>
       <c r="AE305" s="2"/>
     </row>
-    <row r="306" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A306" s="1">
         <v>248</v>
       </c>
@@ -30959,7 +30959,7 @@
       </c>
       <c r="AE306" s="2"/>
     </row>
-    <row r="307" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A307" s="1">
         <v>249</v>
       </c>
@@ -31052,7 +31052,7 @@
       </c>
       <c r="AE307" s="2"/>
     </row>
-    <row r="308" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A308" s="1">
         <v>250</v>
       </c>
@@ -31145,7 +31145,7 @@
       </c>
       <c r="AE308" s="2"/>
     </row>
-    <row r="309" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A309" s="1">
         <v>251</v>
       </c>
@@ -31238,7 +31238,7 @@
       </c>
       <c r="AE309" s="2"/>
     </row>
-    <row r="310" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A310" s="1">
         <v>251</v>
       </c>
@@ -31331,7 +31331,7 @@
       </c>
       <c r="AE310" s="2"/>
     </row>
-    <row r="311" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A311" s="1">
         <v>251</v>
       </c>
@@ -31424,7 +31424,7 @@
       </c>
       <c r="AE311" s="2"/>
     </row>
-    <row r="312" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A312" s="1">
         <v>252</v>
       </c>
@@ -31517,7 +31517,7 @@
       </c>
       <c r="AE312" s="2"/>
     </row>
-    <row r="313" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A313" s="1">
         <v>252</v>
       </c>
@@ -31610,7 +31610,7 @@
       </c>
       <c r="AE313" s="2"/>
     </row>
-    <row r="314" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A314" s="1">
         <v>252</v>
       </c>
@@ -31703,7 +31703,7 @@
       </c>
       <c r="AE314" s="2"/>
     </row>
-    <row r="315" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A315" s="1">
         <v>253</v>
       </c>
@@ -31796,7 +31796,7 @@
       </c>
       <c r="AE315" s="2"/>
     </row>
-    <row r="316" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A316" s="1">
         <v>254</v>
       </c>
@@ -31889,7 +31889,7 @@
       </c>
       <c r="AE316" s="2"/>
     </row>
-    <row r="317" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A317" s="1">
         <v>255</v>
       </c>
@@ -31982,7 +31982,7 @@
       </c>
       <c r="AE317" s="2"/>
     </row>
-    <row r="318" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A318" s="1">
         <v>256</v>
       </c>
@@ -32075,7 +32075,7 @@
       </c>
       <c r="AE318" s="2"/>
     </row>
-    <row r="319" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A319" s="1">
         <v>257</v>
       </c>
@@ -32168,7 +32168,7 @@
       </c>
       <c r="AE319" s="2"/>
     </row>
-    <row r="320" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A320" s="1">
         <v>258</v>
       </c>
@@ -32261,7 +32261,7 @@
       </c>
       <c r="AE320" s="2"/>
     </row>
-    <row r="321" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A321" s="1">
         <v>259</v>
       </c>
@@ -32354,7 +32354,7 @@
       </c>
       <c r="AE321" s="2"/>
     </row>
-    <row r="322" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A322" s="1">
         <v>260</v>
       </c>
@@ -32447,7 +32447,7 @@
       </c>
       <c r="AE322" s="2"/>
     </row>
-    <row r="323" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A323" s="1">
         <v>261</v>
       </c>
@@ -32540,7 +32540,7 @@
       </c>
       <c r="AE323" s="2"/>
     </row>
-    <row r="324" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A324" s="1">
         <v>262</v>
       </c>
@@ -32633,7 +32633,7 @@
       </c>
       <c r="AE324" s="2"/>
     </row>
-    <row r="325" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A325" s="1">
         <v>263</v>
       </c>
@@ -32726,7 +32726,7 @@
       </c>
       <c r="AE325" s="2"/>
     </row>
-    <row r="326" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A326" s="1">
         <v>264</v>
       </c>
@@ -32819,7 +32819,7 @@
       </c>
       <c r="AE326" s="2"/>
     </row>
-    <row r="327" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A327" s="1">
         <v>265</v>
       </c>
@@ -32912,7 +32912,7 @@
       </c>
       <c r="AE327" s="2"/>
     </row>
-    <row r="328" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A328" s="1">
         <v>266</v>
       </c>
@@ -33005,7 +33005,7 @@
       </c>
       <c r="AE328" s="2"/>
     </row>
-    <row r="329" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A329" s="1">
         <v>267</v>
       </c>
@@ -33098,7 +33098,7 @@
       </c>
       <c r="AE329" s="2"/>
     </row>
-    <row r="330" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A330" s="1">
         <v>268</v>
       </c>
@@ -33191,7 +33191,7 @@
       </c>
       <c r="AE330" s="2"/>
     </row>
-    <row r="331" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A331" s="1">
         <v>268</v>
       </c>
@@ -33284,7 +33284,7 @@
       </c>
       <c r="AE331" s="2"/>
     </row>
-    <row r="332" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A332" s="1">
         <v>268</v>
       </c>
@@ -33377,7 +33377,7 @@
       </c>
       <c r="AE332" s="2"/>
     </row>
-    <row r="333" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A333" s="1">
         <v>269</v>
       </c>
@@ -33470,7 +33470,7 @@
       </c>
       <c r="AE333" s="2"/>
     </row>
-    <row r="334" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A334" s="1">
         <v>270</v>
       </c>
@@ -33563,7 +33563,7 @@
       </c>
       <c r="AE334" s="2"/>
     </row>
-    <row r="335" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A335" s="1">
         <v>271</v>
       </c>
@@ -33656,7 +33656,7 @@
       </c>
       <c r="AE335" s="2"/>
     </row>
-    <row r="336" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A336" s="1">
         <v>271</v>
       </c>
@@ -33749,7 +33749,7 @@
       </c>
       <c r="AE336" s="2"/>
     </row>
-    <row r="337" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A337" s="1">
         <v>271</v>
       </c>
@@ -33842,7 +33842,7 @@
       </c>
       <c r="AE337" s="2"/>
     </row>
-    <row r="338" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A338" s="1">
         <v>272</v>
       </c>
@@ -33935,7 +33935,7 @@
       </c>
       <c r="AE338" s="2"/>
     </row>
-    <row r="339" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A339" s="1">
         <v>273</v>
       </c>
@@ -34028,7 +34028,7 @@
       </c>
       <c r="AE339" s="2"/>
     </row>
-    <row r="340" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A340" s="1">
         <v>273</v>
       </c>
@@ -34121,7 +34121,7 @@
       </c>
       <c r="AE340" s="2"/>
     </row>
-    <row r="341" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A341" s="1">
         <v>273</v>
       </c>
@@ -34214,7 +34214,7 @@
       </c>
       <c r="AE341" s="2"/>
     </row>
-    <row r="342" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A342" s="1">
         <v>274</v>
       </c>
@@ -34307,7 +34307,7 @@
       </c>
       <c r="AE342" s="2"/>
     </row>
-    <row r="343" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A343" s="1">
         <v>274</v>
       </c>
@@ -34400,7 +34400,7 @@
       </c>
       <c r="AE343" s="2"/>
     </row>
-    <row r="344" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A344" s="1">
         <v>274</v>
       </c>
@@ -34493,7 +34493,7 @@
       </c>
       <c r="AE344" s="2"/>
     </row>
-    <row r="345" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A345" s="1">
         <v>275</v>
       </c>
@@ -34586,7 +34586,7 @@
       </c>
       <c r="AE345" s="2"/>
     </row>
-    <row r="346" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A346" s="1">
         <v>275</v>
       </c>
@@ -34679,7 +34679,7 @@
       </c>
       <c r="AE346" s="2"/>
     </row>
-    <row r="347" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A347" s="1">
         <v>275</v>
       </c>
@@ -34772,7 +34772,7 @@
       </c>
       <c r="AE347" s="2"/>
     </row>
-    <row r="348" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A348" s="1">
         <v>276</v>
       </c>
@@ -34865,7 +34865,7 @@
       </c>
       <c r="AE348" s="2"/>
     </row>
-    <row r="349" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A349" s="1">
         <v>277</v>
       </c>
@@ -34958,7 +34958,7 @@
       </c>
       <c r="AE349" s="2"/>
     </row>
-    <row r="350" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A350" s="1">
         <v>278</v>
       </c>
@@ -35051,7 +35051,7 @@
       </c>
       <c r="AE350" s="2"/>
     </row>
-    <row r="351" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A351" s="1">
         <v>279</v>
       </c>
@@ -35144,7 +35144,7 @@
       </c>
       <c r="AE351" s="2"/>
     </row>
-    <row r="352" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A352" s="1">
         <v>279</v>
       </c>
@@ -35237,7 +35237,7 @@
       </c>
       <c r="AE352" s="2"/>
     </row>
-    <row r="353" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A353" s="1">
         <v>279</v>
       </c>
@@ -35330,7 +35330,7 @@
       </c>
       <c r="AE353" s="2"/>
     </row>
-    <row r="354" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A354" s="1">
         <v>280</v>
       </c>
@@ -35423,7 +35423,7 @@
       </c>
       <c r="AE354" s="2"/>
     </row>
-    <row r="355" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A355" s="1">
         <v>281</v>
       </c>
@@ -35516,7 +35516,7 @@
       </c>
       <c r="AE355" s="2"/>
     </row>
-    <row r="356" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A356" s="1">
         <v>282</v>
       </c>
@@ -35609,7 +35609,7 @@
       </c>
       <c r="AE356" s="2"/>
     </row>
-    <row r="357" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A357" s="1">
         <v>282</v>
       </c>
@@ -35700,7 +35700,7 @@
       </c>
       <c r="AE357" s="2"/>
     </row>
-    <row r="358" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
         <v>282</v>
       </c>
@@ -35791,7 +35791,7 @@
       </c>
       <c r="AE358" s="2"/>
     </row>
-    <row r="359" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A359" s="1">
         <v>282</v>
       </c>
@@ -35884,7 +35884,7 @@
       </c>
       <c r="AE359" s="2"/>
     </row>
-    <row r="360" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A360" s="1">
         <v>283</v>
       </c>
@@ -35975,7 +35975,7 @@
       </c>
       <c r="AE360" s="2"/>
     </row>
-    <row r="361" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A361" s="1">
         <v>283</v>
       </c>
@@ -36066,7 +36066,7 @@
       </c>
       <c r="AE361" s="2"/>
     </row>
-    <row r="362" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A362" s="1">
         <v>283</v>
       </c>
@@ -36157,7 +36157,7 @@
       </c>
       <c r="AE362" s="2"/>
     </row>
-    <row r="363" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A363" s="1">
         <v>284</v>
       </c>
@@ -36252,7 +36252,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="364" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A364" s="1">
         <v>285</v>
       </c>
@@ -36345,7 +36345,7 @@
       </c>
       <c r="AE364" s="2"/>
     </row>
-    <row r="365" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A365" s="1">
         <v>286</v>
       </c>
@@ -36438,7 +36438,7 @@
       </c>
       <c r="AE365" s="2"/>
     </row>
-    <row r="366" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A366" s="1">
         <v>287</v>
       </c>
@@ -36531,7 +36531,7 @@
       </c>
       <c r="AE366" s="2"/>
     </row>
-    <row r="367" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
         <v>288</v>
       </c>
@@ -36624,7 +36624,7 @@
       </c>
       <c r="AE367" s="2"/>
     </row>
-    <row r="368" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A368" s="1">
         <v>288</v>
       </c>
@@ -36717,7 +36717,7 @@
       </c>
       <c r="AE368" s="2"/>
     </row>
-    <row r="369" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A369" s="1">
         <v>288</v>
       </c>
@@ -36810,7 +36810,7 @@
       </c>
       <c r="AE369" s="2"/>
     </row>
-    <row r="370" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A370" s="1">
         <v>289</v>
       </c>
@@ -36903,7 +36903,7 @@
       </c>
       <c r="AE370" s="2"/>
     </row>
-    <row r="371" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A371" s="1">
         <v>289</v>
       </c>
@@ -36996,7 +36996,7 @@
       </c>
       <c r="AE371" s="2"/>
     </row>
-    <row r="372" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A372" s="1">
         <v>289</v>
       </c>
@@ -37089,7 +37089,7 @@
       </c>
       <c r="AE372" s="2"/>
     </row>
-    <row r="373" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A373" s="1">
         <v>289</v>
       </c>
@@ -37182,7 +37182,7 @@
       </c>
       <c r="AE373" s="2"/>
     </row>
-    <row r="374" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A374" s="1">
         <v>290</v>
       </c>
@@ -37275,7 +37275,7 @@
       </c>
       <c r="AE374" s="2"/>
     </row>
-    <row r="375" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A375" s="1">
         <v>291</v>
       </c>
@@ -37368,7 +37368,7 @@
       </c>
       <c r="AE375" s="2"/>
     </row>
-    <row r="376" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A376" s="1">
         <v>291</v>
       </c>
@@ -37461,7 +37461,7 @@
       </c>
       <c r="AE376" s="2"/>
     </row>
-    <row r="377" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A377" s="1">
         <v>291</v>
       </c>
@@ -37554,7 +37554,7 @@
       </c>
       <c r="AE377" s="2"/>
     </row>
-    <row r="378" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A378" s="1">
         <v>292</v>
       </c>
@@ -37647,7 +37647,7 @@
       </c>
       <c r="AE378" s="2"/>
     </row>
-    <row r="379" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A379" s="1">
         <v>293</v>
       </c>
@@ -37740,7 +37740,7 @@
       </c>
       <c r="AE379" s="2"/>
     </row>
-    <row r="380" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A380" s="1">
         <v>294</v>
       </c>
@@ -37833,7 +37833,7 @@
       </c>
       <c r="AE380" s="2"/>
     </row>
-    <row r="381" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A381" s="1">
         <v>295</v>
       </c>
@@ -37926,7 +37926,7 @@
       </c>
       <c r="AE381" s="2"/>
     </row>
-    <row r="382" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A382" s="1">
         <v>296</v>
       </c>
@@ -38019,7 +38019,7 @@
       </c>
       <c r="AE382" s="2"/>
     </row>
-    <row r="383" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A383" s="1">
         <v>297</v>
       </c>
@@ -38112,7 +38112,7 @@
       </c>
       <c r="AE383" s="2"/>
     </row>
-    <row r="384" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A384" s="1">
         <v>297</v>
       </c>
@@ -38205,7 +38205,7 @@
       </c>
       <c r="AE384" s="2"/>
     </row>
-    <row r="385" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A385" s="1">
         <v>297</v>
       </c>
@@ -38298,7 +38298,7 @@
       </c>
       <c r="AE385" s="2"/>
     </row>
-    <row r="386" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A386" s="1">
         <v>298</v>
       </c>
@@ -38391,7 +38391,7 @@
       </c>
       <c r="AE386" s="2"/>
     </row>
-    <row r="387" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A387" s="1">
         <v>298</v>
       </c>
@@ -38484,7 +38484,7 @@
       </c>
       <c r="AE387" s="2"/>
     </row>
-    <row r="388" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A388" s="1">
         <v>298</v>
       </c>
@@ -38577,7 +38577,7 @@
       </c>
       <c r="AE388" s="2"/>
     </row>
-    <row r="389" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A389" s="1">
         <v>299</v>
       </c>
@@ -38670,7 +38670,7 @@
       </c>
       <c r="AE389" s="2"/>
     </row>
-    <row r="390" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A390" s="1">
         <v>300</v>
       </c>
@@ -38763,7 +38763,7 @@
       </c>
       <c r="AE390" s="2"/>
     </row>
-    <row r="391" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A391" s="1">
         <v>301</v>
       </c>
@@ -38856,7 +38856,7 @@
       </c>
       <c r="AE391" s="2"/>
     </row>
-    <row r="392" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A392" s="1">
         <v>302</v>
       </c>
@@ -38949,7 +38949,7 @@
       </c>
       <c r="AE392" s="2"/>
     </row>
-    <row r="393" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A393" s="1">
         <v>303</v>
       </c>
@@ -39042,7 +39042,7 @@
       </c>
       <c r="AE393" s="2"/>
     </row>
-    <row r="394" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A394" s="1">
         <v>304</v>
       </c>
@@ -39135,7 +39135,7 @@
       </c>
       <c r="AE394" s="2"/>
     </row>
-    <row r="395" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A395" s="1">
         <v>304</v>
       </c>
@@ -39228,7 +39228,7 @@
       </c>
       <c r="AE395" s="2"/>
     </row>
-    <row r="396" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A396" s="1">
         <v>304</v>
       </c>
@@ -39321,7 +39321,7 @@
       </c>
       <c r="AE396" s="2"/>
     </row>
-    <row r="397" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A397" s="1">
         <v>305</v>
       </c>
@@ -39414,7 +39414,7 @@
       </c>
       <c r="AE397" s="2"/>
     </row>
-    <row r="398" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A398" s="1">
         <v>306</v>
       </c>
@@ -39507,7 +39507,7 @@
       </c>
       <c r="AE398" s="2"/>
     </row>
-    <row r="399" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A399" s="1">
         <v>307</v>
       </c>
@@ -39600,7 +39600,7 @@
       </c>
       <c r="AE399" s="2"/>
     </row>
-    <row r="400" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A400" s="1">
         <v>308</v>
       </c>
@@ -39693,7 +39693,7 @@
       </c>
       <c r="AE400" s="2"/>
     </row>
-    <row r="401" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A401" s="1">
         <v>309</v>
       </c>
@@ -39786,7 +39786,7 @@
       </c>
       <c r="AE401" s="2"/>
     </row>
-    <row r="402" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A402" s="1">
         <v>309</v>
       </c>
@@ -39879,7 +39879,7 @@
       </c>
       <c r="AE402" s="2"/>
     </row>
-    <row r="403" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A403" s="1">
         <v>309</v>
       </c>
@@ -39972,7 +39972,7 @@
       </c>
       <c r="AE403" s="2"/>
     </row>
-    <row r="404" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A404" s="1">
         <v>310</v>
       </c>
@@ -40065,7 +40065,7 @@
       </c>
       <c r="AE404" s="2"/>
     </row>
-    <row r="405" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A405" s="1">
         <v>311</v>
       </c>
@@ -40158,7 +40158,7 @@
       </c>
       <c r="AE405" s="2"/>
     </row>
-    <row r="406" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A406" s="1">
         <v>312</v>
       </c>
@@ -40251,7 +40251,7 @@
       </c>
       <c r="AE406" s="2"/>
     </row>
-    <row r="407" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A407" s="1">
         <v>313</v>
       </c>
@@ -40344,7 +40344,7 @@
       </c>
       <c r="AE407" s="2"/>
     </row>
-    <row r="408" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A408" s="1">
         <v>314</v>
       </c>
@@ -40437,7 +40437,7 @@
       </c>
       <c r="AE408" s="2"/>
     </row>
-    <row r="409" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A409" s="1">
         <v>314</v>
       </c>
@@ -40530,7 +40530,7 @@
       </c>
       <c r="AE409" s="2"/>
     </row>
-    <row r="410" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A410" s="1">
         <v>314</v>
       </c>
@@ -40623,7 +40623,7 @@
       </c>
       <c r="AE410" s="2"/>
     </row>
-    <row r="411" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A411" s="1">
         <v>315</v>
       </c>
@@ -40716,7 +40716,7 @@
       </c>
       <c r="AE411" s="2"/>
     </row>
-    <row r="412" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A412" s="1">
         <v>316</v>
       </c>
@@ -40809,7 +40809,7 @@
       </c>
       <c r="AE412" s="2"/>
     </row>
-    <row r="413" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A413" s="1">
         <v>317</v>
       </c>
@@ -40902,7 +40902,7 @@
       </c>
       <c r="AE413" s="2"/>
     </row>
-    <row r="414" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A414" s="1">
         <v>318</v>
       </c>
@@ -40995,7 +40995,7 @@
       </c>
       <c r="AE414" s="2"/>
     </row>
-    <row r="415" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A415" s="1">
         <v>319</v>
       </c>
@@ -41088,7 +41088,7 @@
       </c>
       <c r="AE415" s="2"/>
     </row>
-    <row r="416" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A416" s="1">
         <v>320</v>
       </c>
@@ -41181,7 +41181,7 @@
       </c>
       <c r="AE416" s="2"/>
     </row>
-    <row r="417" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A417" s="1">
         <v>321</v>
       </c>
@@ -41274,7 +41274,7 @@
       </c>
       <c r="AE417" s="2"/>
     </row>
-    <row r="418" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A418" s="1">
         <v>322</v>
       </c>
@@ -41367,7 +41367,7 @@
       </c>
       <c r="AE418" s="2"/>
     </row>
-    <row r="419" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A419" s="1">
         <v>323</v>
       </c>
@@ -41462,7 +41462,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="420" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A420" s="1">
         <v>324</v>
       </c>
@@ -41555,7 +41555,7 @@
       </c>
       <c r="AE420" s="2"/>
     </row>
-    <row r="421" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A421" s="1">
         <v>325</v>
       </c>
@@ -41648,7 +41648,7 @@
       </c>
       <c r="AE421" s="2"/>
     </row>
-    <row r="422" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A422" s="1">
         <v>326</v>
       </c>
@@ -41741,7 +41741,7 @@
       </c>
       <c r="AE422" s="2"/>
     </row>
-    <row r="423" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A423" s="1">
         <v>327</v>
       </c>
@@ -41834,7 +41834,7 @@
       </c>
       <c r="AE423" s="2"/>
     </row>
-    <row r="424" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A424" s="1">
         <v>328</v>
       </c>
@@ -41927,7 +41927,7 @@
       </c>
       <c r="AE424" s="2"/>
     </row>
-    <row r="425" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A425" s="1">
         <v>329</v>
       </c>
@@ -42020,7 +42020,7 @@
       </c>
       <c r="AE425" s="2"/>
     </row>
-    <row r="426" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A426" s="1">
         <v>330</v>
       </c>
@@ -42113,7 +42113,7 @@
       </c>
       <c r="AE426" s="2"/>
     </row>
-    <row r="427" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A427" s="1">
         <v>331</v>
       </c>
@@ -42206,7 +42206,7 @@
       </c>
       <c r="AE427" s="2"/>
     </row>
-    <row r="428" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A428" s="1">
         <v>332</v>
       </c>
@@ -42299,7 +42299,7 @@
       </c>
       <c r="AE428" s="2"/>
     </row>
-    <row r="429" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A429" s="1">
         <v>333</v>
       </c>
@@ -42392,7 +42392,7 @@
       </c>
       <c r="AE429" s="2"/>
     </row>
-    <row r="430" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A430" s="1">
         <v>334</v>
       </c>
@@ -42485,7 +42485,7 @@
       </c>
       <c r="AE430" s="2"/>
     </row>
-    <row r="431" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A431" s="1">
         <v>335</v>
       </c>
@@ -42578,7 +42578,7 @@
       </c>
       <c r="AE431" s="2"/>
     </row>
-    <row r="432" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A432" s="1">
         <v>335</v>
       </c>
@@ -42671,7 +42671,7 @@
       </c>
       <c r="AE432" s="2"/>
     </row>
-    <row r="433" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A433" s="1">
         <v>335</v>
       </c>
@@ -42764,7 +42764,7 @@
       </c>
       <c r="AE433" s="2"/>
     </row>
-    <row r="434" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A434" s="1">
         <v>336</v>
       </c>
@@ -42855,7 +42855,7 @@
       </c>
       <c r="AE434" s="2"/>
     </row>
-    <row r="435" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A435" s="1">
         <v>337</v>
       </c>
@@ -42946,7 +42946,7 @@
       </c>
       <c r="AE435" s="2"/>
     </row>
-    <row r="436" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A436" s="1">
         <v>338</v>
       </c>
@@ -43039,7 +43039,7 @@
       </c>
       <c r="AE436" s="2"/>
     </row>
-    <row r="437" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A437" s="1">
         <v>339</v>
       </c>
@@ -43132,7 +43132,7 @@
       </c>
       <c r="AE437" s="2"/>
     </row>
-    <row r="438" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A438" s="1">
         <v>340</v>
       </c>
@@ -43225,7 +43225,7 @@
       </c>
       <c r="AE438" s="2"/>
     </row>
-    <row r="439" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A439" s="1">
         <v>340</v>
       </c>
@@ -43318,7 +43318,7 @@
       </c>
       <c r="AE439" s="2"/>
     </row>
-    <row r="440" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A440" s="1">
         <v>340</v>
       </c>
@@ -43411,7 +43411,7 @@
       </c>
       <c r="AE440" s="2"/>
     </row>
-    <row r="441" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A441" s="1">
         <v>341</v>
       </c>
@@ -43504,7 +43504,7 @@
       </c>
       <c r="AE441" s="2"/>
     </row>
-    <row r="442" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A442" s="1">
         <v>341</v>
       </c>
@@ -43597,7 +43597,7 @@
       </c>
       <c r="AE442" s="2"/>
     </row>
-    <row r="443" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A443" s="1">
         <v>341</v>
       </c>
@@ -43690,7 +43690,7 @@
       </c>
       <c r="AE443" s="2"/>
     </row>
-    <row r="444" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A444" s="1">
         <v>342</v>
       </c>
@@ -43783,7 +43783,7 @@
       </c>
       <c r="AE444" s="2"/>
     </row>
-    <row r="445" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A445" s="1">
         <v>342</v>
       </c>
@@ -43874,7 +43874,7 @@
       </c>
       <c r="AE445" s="2"/>
     </row>
-    <row r="446" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A446" s="1">
         <v>342</v>
       </c>
@@ -43967,7 +43967,7 @@
       </c>
       <c r="AE446" s="2"/>
     </row>
-    <row r="447" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A447" s="1">
         <v>343</v>
       </c>
@@ -44060,7 +44060,7 @@
       </c>
       <c r="AE447" s="2"/>
     </row>
-    <row r="448" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A448" s="1">
         <v>344</v>
       </c>
@@ -44153,7 +44153,7 @@
       </c>
       <c r="AE448" s="2"/>
     </row>
-    <row r="449" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A449" s="1">
         <v>345</v>
       </c>
@@ -44246,7 +44246,7 @@
       </c>
       <c r="AE449" s="2"/>
     </row>
-    <row r="450" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A450" s="1">
         <v>346</v>
       </c>
@@ -44339,7 +44339,7 @@
       </c>
       <c r="AE450" s="2"/>
     </row>
-    <row r="451" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A451" s="1">
         <v>346</v>
       </c>
@@ -44432,7 +44432,7 @@
       </c>
       <c r="AE451" s="2"/>
     </row>
-    <row r="452" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A452" s="1">
         <v>346</v>
       </c>
@@ -44525,7 +44525,7 @@
       </c>
       <c r="AE452" s="2"/>
     </row>
-    <row r="453" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A453" s="1">
         <v>347</v>
       </c>
@@ -44618,7 +44618,7 @@
       </c>
       <c r="AE453" s="2"/>
     </row>
-    <row r="454" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A454" s="1">
         <v>348</v>
       </c>
@@ -44711,7 +44711,7 @@
       </c>
       <c r="AE454" s="2"/>
     </row>
-    <row r="455" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A455" s="1">
         <v>349</v>
       </c>
@@ -44804,7 +44804,7 @@
       </c>
       <c r="AE455" s="2"/>
     </row>
-    <row r="456" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A456" s="1">
         <v>350</v>
       </c>
@@ -44897,7 +44897,7 @@
       </c>
       <c r="AE456" s="2"/>
     </row>
-    <row r="457" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A457" s="1">
         <v>351</v>
       </c>
@@ -44990,7 +44990,7 @@
       </c>
       <c r="AE457" s="2"/>
     </row>
-    <row r="458" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A458" s="1">
         <v>352</v>
       </c>
@@ -45083,7 +45083,7 @@
       </c>
       <c r="AE458" s="2"/>
     </row>
-    <row r="459" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A459" s="1">
         <v>353</v>
       </c>
@@ -45176,7 +45176,7 @@
       </c>
       <c r="AE459" s="2"/>
     </row>
-    <row r="460" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A460" s="1">
         <v>354</v>
       </c>
@@ -45269,7 +45269,7 @@
       </c>
       <c r="AE460" s="2"/>
     </row>
-    <row r="461" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A461" s="1">
         <v>354</v>
       </c>
@@ -45362,7 +45362,7 @@
       </c>
       <c r="AE461" s="2"/>
     </row>
-    <row r="462" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A462" s="1">
         <v>354</v>
       </c>
@@ -45455,7 +45455,7 @@
       </c>
       <c r="AE462" s="2"/>
     </row>
-    <row r="463" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A463" s="1">
         <v>355</v>
       </c>
@@ -45548,7 +45548,7 @@
       </c>
       <c r="AE463" s="2"/>
     </row>
-    <row r="464" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A464" s="1">
         <v>356</v>
       </c>
@@ -45641,7 +45641,7 @@
       </c>
       <c r="AE464" s="2"/>
     </row>
-    <row r="465" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A465" s="1">
         <v>357</v>
       </c>
@@ -45734,7 +45734,7 @@
       </c>
       <c r="AE465" s="2"/>
     </row>
-    <row r="466" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A466" s="1">
         <v>358</v>
       </c>
@@ -45827,7 +45827,7 @@
       </c>
       <c r="AE466" s="2"/>
     </row>
-    <row r="467" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A467" s="1">
         <v>359</v>
       </c>
@@ -45920,7 +45920,7 @@
       </c>
       <c r="AE467" s="2"/>
     </row>
-    <row r="468" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A468" s="1">
         <v>359</v>
       </c>
@@ -46013,7 +46013,7 @@
       </c>
       <c r="AE468" s="2"/>
     </row>
-    <row r="469" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A469" s="1">
         <v>359</v>
       </c>
@@ -46106,7 +46106,7 @@
       </c>
       <c r="AE469" s="2"/>
     </row>
-    <row r="470" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A470" s="1">
         <v>360</v>
       </c>
@@ -46199,7 +46199,7 @@
       </c>
       <c r="AE470" s="2"/>
     </row>
-    <row r="471" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A471" s="1">
         <v>360</v>
       </c>
@@ -46292,7 +46292,7 @@
       </c>
       <c r="AE471" s="2"/>
     </row>
-    <row r="472" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A472" s="1">
         <v>360</v>
       </c>
@@ -46385,7 +46385,7 @@
       </c>
       <c r="AE472" s="2"/>
     </row>
-    <row r="473" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A473" s="1">
         <v>361</v>
       </c>
@@ -46478,7 +46478,7 @@
       </c>
       <c r="AE473" s="2"/>
     </row>
-    <row r="474" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A474" s="1">
         <v>362</v>
       </c>
@@ -46571,7 +46571,7 @@
       </c>
       <c r="AE474" s="2"/>
     </row>
-    <row r="475" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A475" s="1">
         <v>363</v>
       </c>
@@ -46664,7 +46664,7 @@
       </c>
       <c r="AE475" s="2"/>
     </row>
-    <row r="476" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A476" s="1">
         <v>364</v>
       </c>
@@ -46757,7 +46757,7 @@
       </c>
       <c r="AE476" s="2"/>
     </row>
-    <row r="477" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A477" s="1">
         <v>364</v>
       </c>
@@ -46848,7 +46848,7 @@
       </c>
       <c r="AE477" s="2"/>
     </row>
-    <row r="478" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A478" s="1">
         <v>364</v>
       </c>
@@ -46941,7 +46941,7 @@
       </c>
       <c r="AE478" s="2"/>
     </row>
-    <row r="479" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A479" s="1">
         <v>365</v>
       </c>
@@ -47034,7 +47034,7 @@
       </c>
       <c r="AE479" s="2"/>
     </row>
-    <row r="480" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A480" s="1">
         <v>366</v>
       </c>
@@ -47127,7 +47127,7 @@
       </c>
       <c r="AE480" s="2"/>
     </row>
-    <row r="481" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A481" s="1">
         <v>367</v>
       </c>
@@ -47220,7 +47220,7 @@
       </c>
       <c r="AE481" s="2"/>
     </row>
-    <row r="482" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A482" s="1">
         <v>368</v>
       </c>
@@ -47313,7 +47313,7 @@
       </c>
       <c r="AE482" s="2"/>
     </row>
-    <row r="483" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A483" s="1">
         <v>369</v>
       </c>
@@ -47406,7 +47406,7 @@
       </c>
       <c r="AE483" s="2"/>
     </row>
-    <row r="484" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A484" s="1">
         <v>370</v>
       </c>
@@ -47499,7 +47499,7 @@
       </c>
       <c r="AE484" s="2"/>
     </row>
-    <row r="485" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A485" s="1">
         <v>371</v>
       </c>
@@ -47592,7 +47592,7 @@
       </c>
       <c r="AE485" s="2"/>
     </row>
-    <row r="486" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A486" s="1">
         <v>372</v>
       </c>
@@ -47685,7 +47685,7 @@
       </c>
       <c r="AE486" s="2"/>
     </row>
-    <row r="487" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A487" s="1">
         <v>373</v>
       </c>
@@ -47778,7 +47778,7 @@
       </c>
       <c r="AE487" s="2"/>
     </row>
-    <row r="488" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A488" s="1">
         <v>374</v>
       </c>
@@ -47871,7 +47871,7 @@
       </c>
       <c r="AE488" s="2"/>
     </row>
-    <row r="489" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A489" s="1">
         <v>375</v>
       </c>
@@ -47964,7 +47964,7 @@
       </c>
       <c r="AE489" s="2"/>
     </row>
-    <row r="490" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A490" s="1">
         <v>375</v>
       </c>
@@ -48053,7 +48053,7 @@
       </c>
       <c r="AE490" s="2"/>
     </row>
-    <row r="491" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A491" s="1">
         <v>375</v>
       </c>
@@ -48146,7 +48146,7 @@
       </c>
       <c r="AE491" s="2"/>
     </row>
-    <row r="492" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A492" s="1">
         <v>376</v>
       </c>
@@ -48239,7 +48239,7 @@
       </c>
       <c r="AE492" s="2"/>
     </row>
-    <row r="493" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A493" s="1">
         <v>377</v>
       </c>
@@ -48332,7 +48332,7 @@
       </c>
       <c r="AE493" s="2"/>
     </row>
-    <row r="494" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A494" s="1">
         <v>378</v>
       </c>
@@ -48425,7 +48425,7 @@
       </c>
       <c r="AE494" s="2"/>
     </row>
-    <row r="495" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A495" s="1">
         <v>379</v>
       </c>
@@ -48518,7 +48518,7 @@
       </c>
       <c r="AE495" s="2"/>
     </row>
-    <row r="496" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A496" s="1">
         <v>380</v>
       </c>
@@ -48611,7 +48611,7 @@
       </c>
       <c r="AE496" s="2"/>
     </row>
-    <row r="497" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A497" s="1">
         <v>381</v>
       </c>
@@ -48704,7 +48704,7 @@
       </c>
       <c r="AE497" s="2"/>
     </row>
-    <row r="498" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="498" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A498" s="1">
         <v>382</v>
       </c>
@@ -48797,7 +48797,7 @@
       </c>
       <c r="AE498" s="2"/>
     </row>
-    <row r="499" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="499" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A499" s="1">
         <v>382</v>
       </c>
@@ -48890,7 +48890,7 @@
       </c>
       <c r="AE499" s="2"/>
     </row>
-    <row r="500" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="500" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A500" s="1">
         <v>382</v>
       </c>
@@ -48981,7 +48981,7 @@
       </c>
       <c r="AE500" s="2"/>
     </row>
-    <row r="501" spans="1:31" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A501" s="1">
         <v>382</v>
       </c>

</xml_diff>